<commit_message>
Corrected Calibration Data Files
</commit_message>
<xml_diff>
--- a/Excel Sheets/calibration_middlepoint_5days.xlsx
+++ b/Excel Sheets/calibration_middlepoint_5days.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kx2\Documents\kxu\Trimic-Gripper-Attachment-Signal-Processing\Excel Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kev\Documents\kxu\CMU\Year 1\Trimic-Gripper-Attachment-Signal-Processing\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FECF2C2-AAFD-4594-8DE1-1BAB44163868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909A00BA-A6E4-44B9-B634-C19FD6387632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20880" xr2:uid="{1CA1A152-691A-4307-8C9B-90C4D44A4A25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1CA1A152-691A-4307-8C9B-90C4D44A4A25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,13 +404,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F62C140-3BAA-470B-A903-E4F69280FD0A}">
   <dimension ref="A1:ET50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:ET10"/>
+    <sheetView tabSelected="1" topLeftCell="DR14" workbookViewId="0">
+      <selection activeCell="EK30" sqref="EK30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>94.088189445164602</v>
       </c>
@@ -862,7 +862,7 @@
         <v>58.437714945206203</v>
       </c>
     </row>
-    <row r="2" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>95.073683793985595</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>59.161622561684098</v>
       </c>
     </row>
-    <row r="3" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>94.6836241352581</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>60.1762006193959</v>
       </c>
     </row>
-    <row r="4" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>93.361953859764697</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>57.659413484909898</v>
       </c>
     </row>
-    <row r="5" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>91.489962012722998</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>56.005272288968698</v>
       </c>
     </row>
-    <row r="6" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>93.595187590895804</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>57.699157289977798</v>
       </c>
     </row>
-    <row r="7" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>94.495666499641999</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>58.9895910918952</v>
       </c>
     </row>
-    <row r="8" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>90.094164645174402</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>55.642903772527902</v>
       </c>
     </row>
-    <row r="9" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>93.546535046306602</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>57.381845189256197</v>
       </c>
     </row>
-    <row r="10" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>93.008846296321593</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>56.995431357270597</v>
       </c>
     </row>
-    <row r="11" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>85.186653213658303</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>63.365479313978199</v>
       </c>
     </row>
-    <row r="12" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>83.9287500386951</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>61.767678255393399</v>
       </c>
     </row>
-    <row r="13" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>83.813885975373594</v>
       </c>
@@ -6286,7 +6286,7 @@
         <v>61.710235185734</v>
       </c>
     </row>
-    <row r="14" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>83.578501829581199</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>62.315108264011599</v>
       </c>
     </row>
-    <row r="15" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>84.218917313155501</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>63.047834693221603</v>
       </c>
     </row>
-    <row r="16" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>84.504323752824106</v>
       </c>
@@ -7642,7 +7642,7 @@
         <v>63.392431634736099</v>
       </c>
     </row>
-    <row r="17" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>83.997534530744801</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>62.476287037966998</v>
       </c>
     </row>
-    <row r="18" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>84.048275170423295</v>
       </c>
@@ -8546,7 +8546,7 @@
         <v>62.593564155045001</v>
       </c>
     </row>
-    <row r="19" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>84.866890149443606</v>
       </c>
@@ -8998,7 +8998,7 @@
         <v>63.849813275340601</v>
       </c>
     </row>
-    <row r="20" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>83.522850883614694</v>
       </c>
@@ -9450,7 +9450,7 @@
         <v>61.375442977225099</v>
       </c>
     </row>
-    <row r="21" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>107.531472655852</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>93.167101615215998</v>
       </c>
     </row>
-    <row r="22" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>107.43231458165801</v>
       </c>
@@ -10354,7 +10354,7 @@
         <v>92.869060668252203</v>
       </c>
     </row>
-    <row r="23" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>107.43782982018701</v>
       </c>
@@ -10806,7 +10806,7 @@
         <v>92.858361188371205</v>
       </c>
     </row>
-    <row r="24" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>107.36225476304</v>
       </c>
@@ -11258,7 +11258,7 @@
         <v>92.698159803276596</v>
       </c>
     </row>
-    <row r="25" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>107.37285340395201</v>
       </c>
@@ -11710,7 +11710,7 @@
         <v>92.7320367346247</v>
       </c>
     </row>
-    <row r="26" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>107.206505756526</v>
       </c>
@@ -12162,7 +12162,7 @@
         <v>92.615598467691896</v>
       </c>
     </row>
-    <row r="27" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>107.313026431381</v>
       </c>
@@ -12614,7 +12614,7 @@
         <v>92.623677164972307</v>
       </c>
     </row>
-    <row r="28" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>107.404200334406</v>
       </c>
@@ -13066,7 +13066,7 @@
         <v>92.902659567962601</v>
       </c>
     </row>
-    <row r="29" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>107.502991246535</v>
       </c>
@@ -13518,7 +13518,7 @@
         <v>93.149887125515207</v>
       </c>
     </row>
-    <row r="30" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>107.464439774765</v>
       </c>
@@ -13970,7 +13970,7 @@
         <v>92.838990614505704</v>
       </c>
     </row>
-    <row r="31" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>93.497215268533196</v>
       </c>
@@ -14422,7 +14422,7 @@
         <v>61.065576038805702</v>
       </c>
     </row>
-    <row r="32" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>93.087756796100805</v>
       </c>
@@ -14874,7 +14874,7 @@
         <v>60.708872133948297</v>
       </c>
     </row>
-    <row r="33" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>93.433862286082899</v>
       </c>
@@ -15326,7 +15326,7 @@
         <v>60.331679804820098</v>
       </c>
     </row>
-    <row r="34" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>93.269246114513294</v>
       </c>
@@ -15778,7 +15778,7 @@
         <v>61.022842525610599</v>
       </c>
     </row>
-    <row r="35" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>93.5677687142514</v>
       </c>
@@ -16230,7 +16230,7 @@
         <v>60.928118770642897</v>
       </c>
     </row>
-    <row r="36" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>93.298382521475602</v>
       </c>
@@ -16682,7 +16682,7 @@
         <v>60.474278098933297</v>
       </c>
     </row>
-    <row r="37" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>93.499940396205801</v>
       </c>
@@ -17134,7 +17134,7 @@
         <v>61.910639240894298</v>
       </c>
     </row>
-    <row r="38" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>93.480283784197596</v>
       </c>
@@ -17586,7 +17586,7 @@
         <v>60.443312928846403</v>
       </c>
     </row>
-    <row r="39" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>93.258161948482396</v>
       </c>
@@ -18038,7 +18038,7 @@
         <v>60.575591880833599</v>
       </c>
     </row>
-    <row r="40" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>93.612693965665201</v>
       </c>
@@ -18490,7 +18490,7 @@
         <v>60.8689360136188</v>
       </c>
     </row>
-    <row r="41" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>92.036301678800697</v>
       </c>
@@ -18942,7 +18942,7 @@
         <v>61.609901499122302</v>
       </c>
     </row>
-    <row r="42" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>92.173940099859905</v>
       </c>
@@ -19394,7 +19394,7 @@
         <v>61.517228593621702</v>
       </c>
     </row>
-    <row r="43" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>91.912042669032104</v>
       </c>
@@ -19846,7 +19846,7 @@
         <v>62.297371762549801</v>
       </c>
     </row>
-    <row r="44" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>92.208689777652296</v>
       </c>
@@ -20298,7 +20298,7 @@
         <v>63.396133723747198</v>
       </c>
     </row>
-    <row r="45" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>91.923261329259802</v>
       </c>
@@ -20750,7 +20750,7 @@
         <v>61.521460563119398</v>
       </c>
     </row>
-    <row r="46" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>92.1232445990521</v>
       </c>
@@ -21202,7 +21202,7 @@
         <v>60.619886708013503</v>
       </c>
     </row>
-    <row r="47" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>92.069001652025804</v>
       </c>
@@ -21654,7 +21654,7 @@
         <v>61.060222225882697</v>
       </c>
     </row>
-    <row r="48" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>92.103792333626203</v>
       </c>
@@ -22106,7 +22106,7 @@
         <v>62.378818544468302</v>
       </c>
     </row>
-    <row r="49" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>92.174344083790402</v>
       </c>
@@ -22558,7 +22558,7 @@
         <v>62.3340031104308</v>
       </c>
     </row>
-    <row r="50" spans="1:150" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>92.022960082300301</v>
       </c>

</xml_diff>